<commit_message>
Added functionality to add bulk data storage
</commit_message>
<xml_diff>
--- a/smartexcel/media/STP-Files/Processed/Combined-Data-Sheet.xlsx
+++ b/smartexcel/media/STP-Files/Processed/Combined-Data-Sheet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1031,6 +1031,44 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>form_8.pdf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Paracetamole</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>34545</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>